<commit_message>
Scripting DPLKKPS001-006 until DPLKKPS001-009
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS001-002 - Kepesertaan - Setup Jenis Parameter Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS001-002 - Kepesertaan - Setup Jenis Parameter Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3569273B-57A1-463A-80D2-4AF22111DCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B489C0CC-8EB2-4C6B-97BF-400719B346AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -226,13 +226,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -550,7 +547,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,273 +578,263 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
     </row>
     <row r="2" spans="1:22" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="6">
         <v>100000</v>
       </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
     </row>
     <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="7">
+      <c r="N4" s="7"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="6">
         <v>150000</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
     </row>
     <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>

</xml_diff>